<commit_message>
Set CRS for points_all_cleaned
</commit_message>
<xml_diff>
--- a/outputs/01_cleaneddata/points_all_cleaned.xlsx
+++ b/outputs/01_cleaneddata/points_all_cleaned.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E343"/>
+  <dimension ref="A1:E340"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5396,14 +5396,14 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Wetland-Polygon</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C280">
-        <v>5744645.53809</v>
+        <v>5744651.68363</v>
       </c>
       <c r="D280">
-        <v>342161.18127</v>
+        <v>342156.22389</v>
       </c>
     </row>
     <row r="281">
@@ -5414,14 +5414,14 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Wetland-Polygon</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C281">
-        <v>5744649.52327</v>
+        <v>5744648.54419</v>
       </c>
       <c r="D281">
-        <v>342157.98949</v>
+        <v>342151.42233</v>
       </c>
     </row>
     <row r="282">
@@ -5432,14 +5432,14 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Wetland-Polygon</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C282">
-        <v>5744644.49751</v>
+        <v>5744654.67183</v>
       </c>
       <c r="D282">
-        <v>342157.42048</v>
+        <v>342150.10474</v>
       </c>
     </row>
     <row r="283">
@@ -5454,10 +5454,10 @@
         </is>
       </c>
       <c r="C283">
-        <v>5744651.68363</v>
+        <v>5744660.59818</v>
       </c>
       <c r="D283">
-        <v>342156.22389</v>
+        <v>342147.7043</v>
       </c>
     </row>
     <row r="284">
@@ -5472,10 +5472,10 @@
         </is>
       </c>
       <c r="C284">
-        <v>5744648.54419</v>
+        <v>5744660.39584</v>
       </c>
       <c r="D284">
-        <v>342151.42233</v>
+        <v>342143.94706</v>
       </c>
     </row>
     <row r="285">
@@ -5490,10 +5490,10 @@
         </is>
       </c>
       <c r="C285">
-        <v>5744654.67183</v>
+        <v>5744668.20258</v>
       </c>
       <c r="D285">
-        <v>342150.10474</v>
+        <v>342148.09476</v>
       </c>
     </row>
     <row r="286">
@@ -5508,10 +5508,10 @@
         </is>
       </c>
       <c r="C286">
-        <v>5744660.59818</v>
+        <v>5744672.0219</v>
       </c>
       <c r="D286">
-        <v>342147.7043</v>
+        <v>342145.69257</v>
       </c>
     </row>
     <row r="287">
@@ -5526,10 +5526,10 @@
         </is>
       </c>
       <c r="C287">
-        <v>5744660.39584</v>
+        <v>5744673.38372</v>
       </c>
       <c r="D287">
-        <v>342143.94706</v>
+        <v>342148.13538</v>
       </c>
     </row>
     <row r="288">
@@ -5544,10 +5544,10 @@
         </is>
       </c>
       <c r="C288">
-        <v>5744668.20258</v>
+        <v>5744673.04186</v>
       </c>
       <c r="D288">
-        <v>342148.09476</v>
+        <v>342139.38959</v>
       </c>
     </row>
     <row r="289">
@@ -5562,10 +5562,10 @@
         </is>
       </c>
       <c r="C289">
-        <v>5744672.0219</v>
+        <v>5744674.23773</v>
       </c>
       <c r="D289">
-        <v>342145.69257</v>
+        <v>342134.98741</v>
       </c>
     </row>
     <row r="290">
@@ -5580,10 +5580,10 @@
         </is>
       </c>
       <c r="C290">
-        <v>5744673.38372</v>
+        <v>5744681.17489</v>
       </c>
       <c r="D290">
-        <v>342148.13538</v>
+        <v>342138.87537</v>
       </c>
     </row>
     <row r="291">
@@ -5598,10 +5598,10 @@
         </is>
       </c>
       <c r="C291">
-        <v>5744673.04186</v>
+        <v>5744684.35105</v>
       </c>
       <c r="D291">
-        <v>342139.38959</v>
+        <v>342136.75798</v>
       </c>
     </row>
     <row r="292">
@@ -5616,10 +5616,10 @@
         </is>
       </c>
       <c r="C292">
-        <v>5744674.23773</v>
+        <v>5744686.9267</v>
       </c>
       <c r="D292">
-        <v>342134.98741</v>
+        <v>342140.40155</v>
       </c>
     </row>
     <row r="293">
@@ -5634,10 +5634,10 @@
         </is>
       </c>
       <c r="C293">
-        <v>5744681.17489</v>
+        <v>5744682.46</v>
       </c>
       <c r="D293">
-        <v>342138.87537</v>
+        <v>342146.39368</v>
       </c>
     </row>
     <row r="294">
@@ -5652,10 +5652,10 @@
         </is>
       </c>
       <c r="C294">
-        <v>5744684.35105</v>
+        <v>5744679.36578</v>
       </c>
       <c r="D294">
-        <v>342136.75798</v>
+        <v>342149.18504</v>
       </c>
     </row>
     <row r="295">
@@ -5670,10 +5670,10 @@
         </is>
       </c>
       <c r="C295">
-        <v>5744686.9267</v>
+        <v>5744679.22758</v>
       </c>
       <c r="D295">
-        <v>342140.40155</v>
+        <v>342152.02155</v>
       </c>
     </row>
     <row r="296">
@@ -5688,10 +5688,10 @@
         </is>
       </c>
       <c r="C296">
-        <v>5744682.46</v>
+        <v>5744679.17065</v>
       </c>
       <c r="D296">
-        <v>342146.39368</v>
+        <v>342155.65301</v>
       </c>
     </row>
     <row r="297">
@@ -5706,10 +5706,10 @@
         </is>
       </c>
       <c r="C297">
-        <v>5744679.36578</v>
+        <v>5744686.19558</v>
       </c>
       <c r="D297">
-        <v>342149.18504</v>
+        <v>342156.12478</v>
       </c>
     </row>
     <row r="298">
@@ -5724,10 +5724,10 @@
         </is>
       </c>
       <c r="C298">
-        <v>5744679.22758</v>
+        <v>5744682.29684</v>
       </c>
       <c r="D298">
-        <v>342152.02155</v>
+        <v>342157.90942</v>
       </c>
     </row>
     <row r="299">
@@ -5742,10 +5742,10 @@
         </is>
       </c>
       <c r="C299">
-        <v>5744679.17065</v>
+        <v>5744680.36088</v>
       </c>
       <c r="D299">
-        <v>342155.65301</v>
+        <v>342164.36465</v>
       </c>
     </row>
     <row r="300">
@@ -5760,10 +5760,10 @@
         </is>
       </c>
       <c r="C300">
-        <v>5744686.19558</v>
+        <v>5744678.0299</v>
       </c>
       <c r="D300">
-        <v>342156.12478</v>
+        <v>342167.08632</v>
       </c>
     </row>
     <row r="301">
@@ -5778,10 +5778,10 @@
         </is>
       </c>
       <c r="C301">
-        <v>5744682.29684</v>
+        <v>5744671.18622</v>
       </c>
       <c r="D301">
-        <v>342157.90942</v>
+        <v>342172.96469</v>
       </c>
     </row>
     <row r="302">
@@ -5796,10 +5796,10 @@
         </is>
       </c>
       <c r="C302">
-        <v>5744680.36088</v>
+        <v>5744671.53157</v>
       </c>
       <c r="D302">
-        <v>342164.36465</v>
+        <v>342176.0012</v>
       </c>
     </row>
     <row r="303">
@@ -5810,14 +5810,14 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C303">
-        <v>5744678.0299</v>
+        <v>5744670.57312</v>
       </c>
       <c r="D303">
-        <v>342167.08632</v>
+        <v>342175.17988</v>
       </c>
     </row>
     <row r="304">
@@ -5828,14 +5828,14 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C304">
-        <v>5744671.18622</v>
+        <v>5744667.80921</v>
       </c>
       <c r="D304">
-        <v>342172.96469</v>
+        <v>342174.40008</v>
       </c>
     </row>
     <row r="305">
@@ -5846,14 +5846,14 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C305">
-        <v>5744671.53157</v>
+        <v>5744663.72539</v>
       </c>
       <c r="D305">
-        <v>342176.0012</v>
+        <v>342173.54522</v>
       </c>
     </row>
     <row r="306">
@@ -5868,10 +5868,10 @@
         </is>
       </c>
       <c r="C306">
-        <v>5744670.57312</v>
+        <v>5744660.02687</v>
       </c>
       <c r="D306">
-        <v>342175.17988</v>
+        <v>342170.81739</v>
       </c>
     </row>
     <row r="307">
@@ -5882,14 +5882,14 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Open Water-Point</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C307">
-        <v>5744667.80921</v>
+        <v>5744662.7242</v>
       </c>
       <c r="D307">
-        <v>342174.40008</v>
+        <v>342174.45521</v>
       </c>
     </row>
     <row r="308">
@@ -5900,14 +5900,14 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Open Water-Point</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C308">
-        <v>5744663.72539</v>
+        <v>5744656.61514</v>
       </c>
       <c r="D308">
-        <v>342173.54522</v>
+        <v>342173.35261</v>
       </c>
     </row>
     <row r="309">
@@ -5918,14 +5918,14 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Open Water-Point</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C309">
-        <v>5744660.02687</v>
+        <v>5744649.4127</v>
       </c>
       <c r="D309">
-        <v>342170.81739</v>
+        <v>342174.26364</v>
       </c>
     </row>
     <row r="310">
@@ -5940,10 +5940,10 @@
         </is>
       </c>
       <c r="C310">
-        <v>5744662.7242</v>
+        <v>5744646.41281</v>
       </c>
       <c r="D310">
-        <v>342174.45521</v>
+        <v>342175.5329</v>
       </c>
     </row>
     <row r="311">
@@ -5958,10 +5958,10 @@
         </is>
       </c>
       <c r="C311">
-        <v>5744656.61514</v>
+        <v>5744638.71121</v>
       </c>
       <c r="D311">
-        <v>342173.35261</v>
+        <v>342168.99142</v>
       </c>
     </row>
     <row r="312">
@@ -5976,10 +5976,10 @@
         </is>
       </c>
       <c r="C312">
-        <v>5744649.4127</v>
+        <v>5744635.11151</v>
       </c>
       <c r="D312">
-        <v>342174.26364</v>
+        <v>342166.80111</v>
       </c>
     </row>
     <row r="313">
@@ -5994,10 +5994,10 @@
         </is>
       </c>
       <c r="C313">
-        <v>5744646.41281</v>
+        <v>5744632.18243</v>
       </c>
       <c r="D313">
-        <v>342175.5329</v>
+        <v>342164.83052</v>
       </c>
     </row>
     <row r="314">
@@ -6012,10 +6012,10 @@
         </is>
       </c>
       <c r="C314">
-        <v>5744638.71121</v>
+        <v>5744628.90752</v>
       </c>
       <c r="D314">
-        <v>342168.99142</v>
+        <v>342157.92493</v>
       </c>
     </row>
     <row r="315">
@@ -6030,10 +6030,10 @@
         </is>
       </c>
       <c r="C315">
-        <v>5744635.11151</v>
+        <v>5744625.39603</v>
       </c>
       <c r="D315">
-        <v>342166.80111</v>
+        <v>342160.03835</v>
       </c>
     </row>
     <row r="316">
@@ -6048,10 +6048,10 @@
         </is>
       </c>
       <c r="C316">
-        <v>5744632.18243</v>
+        <v>5744622.35752</v>
       </c>
       <c r="D316">
-        <v>342164.83052</v>
+        <v>342162.21011</v>
       </c>
     </row>
     <row r="317">
@@ -6066,10 +6066,10 @@
         </is>
       </c>
       <c r="C317">
-        <v>5744628.90752</v>
+        <v>5744619.05762</v>
       </c>
       <c r="D317">
-        <v>342157.92493</v>
+        <v>342162.86</v>
       </c>
     </row>
     <row r="318">
@@ -6084,10 +6084,10 @@
         </is>
       </c>
       <c r="C318">
-        <v>5744625.39603</v>
+        <v>5744617.10197</v>
       </c>
       <c r="D318">
-        <v>342160.03835</v>
+        <v>342160.33333</v>
       </c>
     </row>
     <row r="319">
@@ -6102,10 +6102,10 @@
         </is>
       </c>
       <c r="C319">
-        <v>5744622.35752</v>
+        <v>5744621.72112</v>
       </c>
       <c r="D319">
-        <v>342162.21011</v>
+        <v>342158.21666</v>
       </c>
     </row>
     <row r="320">
@@ -6120,10 +6120,10 @@
         </is>
       </c>
       <c r="C320">
-        <v>5744619.05762</v>
+        <v>5744623.74201</v>
       </c>
       <c r="D320">
-        <v>342162.86</v>
+        <v>342154.99166</v>
       </c>
     </row>
     <row r="321">
@@ -6134,14 +6134,14 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C321">
-        <v>5744617.10197</v>
+        <v>5744625.76315</v>
       </c>
       <c r="D321">
-        <v>342160.33333</v>
+        <v>342153.41723</v>
       </c>
     </row>
     <row r="322">
@@ -6156,10 +6156,10 @@
         </is>
       </c>
       <c r="C322">
-        <v>5744621.72112</v>
+        <v>5744629.19395</v>
       </c>
       <c r="D322">
-        <v>342158.21666</v>
+        <v>342158.37088</v>
       </c>
     </row>
     <row r="323">
@@ -6174,10 +6174,10 @@
         </is>
       </c>
       <c r="C323">
-        <v>5744623.74201</v>
+        <v>5744625.2475</v>
       </c>
       <c r="D323">
-        <v>342154.99166</v>
+        <v>342164.78271</v>
       </c>
     </row>
     <row r="324">
@@ -6188,14 +6188,14 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Open Water-Point</t>
+          <t>Wetland-Point</t>
         </is>
       </c>
       <c r="C324">
-        <v>5744625.76315</v>
+        <v>5744622.60671</v>
       </c>
       <c r="D324">
-        <v>342153.41723</v>
+        <v>342163.4501</v>
       </c>
     </row>
     <row r="325">
@@ -6210,10 +6210,10 @@
         </is>
       </c>
       <c r="C325">
-        <v>5744629.19395</v>
+        <v>5744620.31198</v>
       </c>
       <c r="D325">
-        <v>342158.37088</v>
+        <v>342163.8702</v>
       </c>
     </row>
     <row r="326">
@@ -6228,10 +6228,10 @@
         </is>
       </c>
       <c r="C326">
-        <v>5744625.2475</v>
+        <v>5744618.08317</v>
       </c>
       <c r="D326">
-        <v>342164.78271</v>
+        <v>342167.30311</v>
       </c>
     </row>
     <row r="327">
@@ -6246,10 +6246,10 @@
         </is>
       </c>
       <c r="C327">
-        <v>5744622.60671</v>
+        <v>5744616.4691</v>
       </c>
       <c r="D327">
-        <v>342163.4501</v>
+        <v>342163.12555</v>
       </c>
     </row>
     <row r="328">
@@ -6264,10 +6264,10 @@
         </is>
       </c>
       <c r="C328">
-        <v>5744620.31198</v>
+        <v>5744612.50905</v>
       </c>
       <c r="D328">
-        <v>342163.8702</v>
+        <v>342163.10641</v>
       </c>
     </row>
     <row r="329">
@@ -6282,10 +6282,10 @@
         </is>
       </c>
       <c r="C329">
-        <v>5744618.08317</v>
+        <v>5744609.68376</v>
       </c>
       <c r="D329">
-        <v>342167.30311</v>
+        <v>342164.72217</v>
       </c>
     </row>
     <row r="330">
@@ -6300,10 +6300,10 @@
         </is>
       </c>
       <c r="C330">
-        <v>5744616.4691</v>
+        <v>5744608.36121</v>
       </c>
       <c r="D330">
-        <v>342163.12555</v>
+        <v>342167.89963</v>
       </c>
     </row>
     <row r="331">
@@ -6318,10 +6318,10 @@
         </is>
       </c>
       <c r="C331">
-        <v>5744612.50905</v>
+        <v>5744607.97417</v>
       </c>
       <c r="D331">
-        <v>342163.10641</v>
+        <v>342172.36009</v>
       </c>
     </row>
     <row r="332">
@@ -6336,10 +6336,10 @@
         </is>
       </c>
       <c r="C332">
-        <v>5744609.68376</v>
+        <v>5744605.7407</v>
       </c>
       <c r="D332">
-        <v>342164.72217</v>
+        <v>342176.90795</v>
       </c>
     </row>
     <row r="333">
@@ -6354,10 +6354,10 @@
         </is>
       </c>
       <c r="C333">
-        <v>5744608.36121</v>
+        <v>5744614.51295</v>
       </c>
       <c r="D333">
-        <v>342167.89963</v>
+        <v>342173.0573</v>
       </c>
     </row>
     <row r="334">
@@ -6372,10 +6372,10 @@
         </is>
       </c>
       <c r="C334">
-        <v>5744607.97417</v>
+        <v>5744617.89802</v>
       </c>
       <c r="D334">
-        <v>342172.36009</v>
+        <v>342166.5203</v>
       </c>
     </row>
     <row r="335">
@@ -6390,10 +6390,10 @@
         </is>
       </c>
       <c r="C335">
-        <v>5744605.7407</v>
+        <v>5744627.86083</v>
       </c>
       <c r="D335">
-        <v>342176.90795</v>
+        <v>342166.47168</v>
       </c>
     </row>
     <row r="336">
@@ -6408,10 +6408,10 @@
         </is>
       </c>
       <c r="C336">
-        <v>5744614.51295</v>
+        <v>5744632.36189</v>
       </c>
       <c r="D336">
-        <v>342173.0573</v>
+        <v>342166.31812</v>
       </c>
     </row>
     <row r="337">
@@ -6422,14 +6422,14 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C337">
-        <v>5744617.89802</v>
+        <v>5744631.31849</v>
       </c>
       <c r="D337">
-        <v>342166.5203</v>
+        <v>342158.81203</v>
       </c>
     </row>
     <row r="338">
@@ -6440,14 +6440,14 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C338">
-        <v>5744627.86083</v>
+        <v>5744632.96287</v>
       </c>
       <c r="D338">
-        <v>342166.47168</v>
+        <v>342156.9379</v>
       </c>
     </row>
     <row r="339">
@@ -6458,14 +6458,14 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Wetland-Point</t>
+          <t>Open Water-Point</t>
         </is>
       </c>
       <c r="C339">
-        <v>5744632.36189</v>
+        <v>5744628.63139</v>
       </c>
       <c r="D339">
-        <v>342166.31812</v>
+        <v>342155.12187</v>
       </c>
     </row>
     <row r="340">
@@ -6480,63 +6480,9 @@
         </is>
       </c>
       <c r="C340">
-        <v>5744631.31849</v>
+        <v>5744626.17237</v>
       </c>
       <c r="D340">
-        <v>342158.81203</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" t="inlineStr">
-        <is>
-          <t>TumTum</t>
-        </is>
-      </c>
-      <c r="B341" t="inlineStr">
-        <is>
-          <t>Open Water-Point</t>
-        </is>
-      </c>
-      <c r="C341">
-        <v>5744632.96287</v>
-      </c>
-      <c r="D341">
-        <v>342156.9379</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342" t="inlineStr">
-        <is>
-          <t>TumTum</t>
-        </is>
-      </c>
-      <c r="B342" t="inlineStr">
-        <is>
-          <t>Open Water-Point</t>
-        </is>
-      </c>
-      <c r="C342">
-        <v>5744628.63139</v>
-      </c>
-      <c r="D342">
-        <v>342155.12187</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343" t="inlineStr">
-        <is>
-          <t>TumTum</t>
-        </is>
-      </c>
-      <c r="B343" t="inlineStr">
-        <is>
-          <t>Open Water-Point</t>
-        </is>
-      </c>
-      <c r="C343">
-        <v>5744626.17237</v>
-      </c>
-      <c r="D343">
         <v>342153.5034</v>
       </c>
     </row>

</xml_diff>